<commit_message>
Turn off AI thinking
</commit_message>
<xml_diff>
--- a/webai/knfile/AI配置.xlsx
+++ b/webai/knfile/AI配置.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\KnoLib\webai\knfile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\KnoLib\webai\knfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C3DC9D-A6B5-4FB7-80BF-3F5DC3495927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8D936F-A891-418F-B4CC-86AEEDC1C78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="配置" sheetId="1" r:id="rId1"/>
@@ -430,22 +430,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.46484375" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -453,7 +453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -461,7 +461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -480,17 +480,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02000C99-72CF-4549-9323-1E31A1D9E2E1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1328125" customWidth="1"/>
-    <col min="2" max="2" width="20.46484375" customWidth="1"/>
+    <col min="1" max="1" width="22.125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -498,15 +498,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>

</xml_diff>